<commit_message>
script for KORA S3 P1
</commit_message>
<xml_diff>
--- a/rmonize/data_proc_elem/DPE_KORA_S3_P2.xlsx
+++ b/rmonize/data_proc_elem/DPE_KORA_S3_P2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28224"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20415"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\perrar\Documents\Perrar\NFDI4Health\Pilot_Datenharmonisierung\DPEs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\use-cases-harmonisation\rmonize\data_proc_elem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D2444BF4-B900-431D-812F-073905862DBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E6C6673-993B-40BA-833E-67B1654FD5E0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,23 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="792" uniqueCount="319">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="792" uniqueCount="320">
   <si>
     <t>Index</t>
   </si>
@@ -75,25 +64,6 @@
   </si>
   <si>
     <t>KORA _S3_P2</t>
-  </si>
-  <si>
-    <t>col_id</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">
-id_creation</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Menlo"/>
-        <charset val="1"/>
-      </rPr>
-      <t> (mandatory)</t>
-    </r>
   </si>
   <si>
     <t>complete</t>
@@ -1035,12 +1005,22 @@
   <si>
     <t>DV850 (tea)</t>
   </si>
+  <si>
+    <t xml:space="preserve">
+id_creation</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>id_creation</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1130,13 +1110,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <i/>
-      <sz val="10"/>
-      <color rgb="FFFF0000"/>
-      <name val="Menlo"/>
-      <charset val="1"/>
-    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -1164,7 +1137,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1230,18 +1203,19 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1521,13 +1495,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
-      <selection activeCell="E104" sqref="E104"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="25.85546875" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="24.7109375" customWidth="1"/>
     <col min="7" max="7" width="24.28515625" customWidth="1"/>
     <col min="8" max="8" width="22.140625" customWidth="1"/>
@@ -1535,7 +1510,7 @@
     <col min="10" max="10" width="25.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1571,3017 +1546,3017 @@
       </c>
       <c r="L1" s="2"/>
     </row>
-    <row r="2" spans="1:12" ht="15">
-      <c r="A2" s="29">
+    <row r="2" spans="1:12" s="34" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="31">
         <v>1</v>
       </c>
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="31"/>
-      <c r="D2" s="30" t="s">
+      <c r="C2" s="33"/>
+      <c r="D2" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="32" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" s="30" t="s">
-        <v>14</v>
-      </c>
-      <c r="G2" s="30" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2" s="31" t="s">
-        <v>15</v>
-      </c>
-      <c r="I2" s="30" t="s">
-        <v>15</v>
-      </c>
-      <c r="J2" s="30" t="s">
-        <v>16</v>
-      </c>
-      <c r="K2" s="29"/>
-    </row>
-    <row r="3" spans="1:12" ht="15">
+      <c r="E2" s="30" t="s">
+        <v>318</v>
+      </c>
+      <c r="F2" s="32" t="s">
+        <v>317</v>
+      </c>
+      <c r="G2" s="32" t="s">
+        <v>319</v>
+      </c>
+      <c r="H2" s="33" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" s="31"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="H3" s="15"/>
       <c r="I3" s="15" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="J3" s="15" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
     </row>
-    <row r="4" spans="1:12" ht="15">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="15">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>23</v>
-      </c>
       <c r="F4" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="H4" s="15"/>
       <c r="I4" s="15" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="J4" s="15" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
     </row>
-    <row r="5" spans="1:12" ht="15">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
       <c r="B5" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>26</v>
-      </c>
       <c r="F5" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="H5" s="15"/>
       <c r="I5" s="15" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="J5" s="15" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="K5" s="15"/>
       <c r="L5" s="15"/>
     </row>
-    <row r="6" spans="1:12" s="28" customFormat="1" ht="30.75">
+    <row r="6" spans="1:12" s="28" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="23">
         <v>5</v>
       </c>
       <c r="B6" s="28" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="23" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" s="2" t="s">
+      <c r="F6" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="H6" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="E6" s="24" t="s">
-        <v>29</v>
-      </c>
-      <c r="F6" s="23" t="s">
-        <v>20</v>
-      </c>
-      <c r="G6" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="H6" s="24" t="s">
-        <v>30</v>
-      </c>
       <c r="I6" s="23" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="J6" s="23" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="K6" s="23"/>
       <c r="L6" s="23"/>
     </row>
-    <row r="7" spans="1:12" ht="15">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>6</v>
       </c>
       <c r="B7" s="17" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H7" s="15"/>
       <c r="I7" s="15" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J7" s="15" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
     </row>
-    <row r="8" spans="1:12" ht="15">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>7</v>
       </c>
       <c r="B8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>35</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>37</v>
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H8" s="15"/>
       <c r="I8" s="15" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J8" s="15" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
     </row>
-    <row r="9" spans="1:12" ht="15">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H9" s="15"/>
       <c r="I9" s="15" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J9" s="15" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
     </row>
-    <row r="10" spans="1:12" ht="30.75">
+    <row r="10" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="15">
         <v>9</v>
       </c>
       <c r="B10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E10" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D10" s="2" t="s">
+      <c r="F10" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H10" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="E10" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="F10" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="H10" s="16" t="s">
-        <v>43</v>
-      </c>
       <c r="I10" s="15" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="J10" s="15" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
     </row>
-    <row r="11" spans="1:12" ht="15">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="15">
         <v>10</v>
       </c>
       <c r="B11" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E11" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C11" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="D11" s="2" t="s">
+      <c r="F11" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H11" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="E11" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="F11" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="H11" s="16" t="s">
-        <v>47</v>
-      </c>
       <c r="I11" s="15" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="J11" s="15" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="K11" s="15"/>
       <c r="L11" s="15"/>
     </row>
-    <row r="12" spans="1:12" ht="15">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="15">
         <v>11</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E12" s="2"/>
       <c r="F12" s="15" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G12" s="16" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H12" s="16" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="I12" s="15" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J12" s="15" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="K12" s="15"/>
       <c r="L12" s="15"/>
     </row>
-    <row r="13" spans="1:12" ht="15">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>12</v>
       </c>
       <c r="B13" t="s">
+        <v>49</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E13" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C13" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>53</v>
-      </c>
       <c r="F13" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="H13" s="15"/>
       <c r="I13" s="15" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="J13" s="15" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="K13" s="15"/>
       <c r="L13" s="15"/>
     </row>
-    <row r="14" spans="1:12" ht="15">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H14" s="15"/>
       <c r="I14" s="15" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J14" s="15" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
     </row>
-    <row r="15" spans="1:12" ht="15">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="15" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G15" s="15" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H15" s="16" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="I15" s="15" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J15" s="15" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="K15" s="2"/>
       <c r="L15" s="2"/>
     </row>
-    <row r="16" spans="1:12" ht="15">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="15">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="15" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G16" s="15" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H16" s="16" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="I16" s="15" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J16" s="15" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="K16" s="2"/>
       <c r="L16" s="2"/>
     </row>
-    <row r="17" spans="1:12" ht="15">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" s="15" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E17" s="2"/>
       <c r="F17" s="15" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G17" s="15" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H17" s="16"/>
       <c r="I17" s="15" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J17" s="15" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="K17" s="15"/>
       <c r="L17" s="15"/>
     </row>
-    <row r="18" spans="1:12" ht="15">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" s="17" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C18" s="17" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E18" s="18"/>
       <c r="F18" s="17" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G18" s="17" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H18" s="19"/>
       <c r="I18" s="17" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J18" s="17" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" ht="15">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E19" s="20"/>
       <c r="F19" s="17" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G19" s="17" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H19" s="20"/>
       <c r="I19" s="17" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J19" s="17" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" ht="15">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C20" t="s">
+        <v>34</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E20" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C20" t="s">
-        <v>36</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>68</v>
-      </c>
       <c r="F20" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="H20" s="1"/>
       <c r="I20" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" ht="15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C21" t="s">
+        <v>34</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E21" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="C21" t="s">
-        <v>36</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>71</v>
-      </c>
       <c r="F21" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="H21" s="1"/>
       <c r="I21" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" ht="15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="C22" t="s">
+        <v>34</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E22" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="C22" t="s">
-        <v>36</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>74</v>
-      </c>
       <c r="F22" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="H22" s="1"/>
       <c r="I22" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" ht="15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="15">
         <v>23</v>
       </c>
       <c r="B23" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="C23" t="s">
+        <v>34</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E23" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="C23" t="s">
-        <v>36</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>77</v>
-      </c>
       <c r="F23" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="H23" s="1"/>
       <c r="I23" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" ht="30.75">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="15">
         <v>24</v>
       </c>
       <c r="B24" t="s">
+        <v>76</v>
+      </c>
+      <c r="C24" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="E24" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="C24" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="E24" s="16" t="s">
-        <v>80</v>
-      </c>
       <c r="F24" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="H24" s="15"/>
       <c r="I24" s="15" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="J24" s="15" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" ht="15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="23">
         <v>25</v>
       </c>
       <c r="B25" t="s">
+        <v>79</v>
+      </c>
+      <c r="C25" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E25" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="C25" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="E25" s="16" t="s">
-        <v>83</v>
-      </c>
       <c r="F25" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="H25" s="15"/>
       <c r="I25" s="15" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="J25" s="15" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" ht="15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="25">
         <v>26</v>
       </c>
       <c r="B26" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C26" s="23" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E26" s="2"/>
       <c r="F26" s="23" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="G26" s="24"/>
       <c r="H26" s="23"/>
       <c r="I26" s="23" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="J26" s="23" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" ht="15">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="15">
         <v>27</v>
       </c>
       <c r="B27" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C27" s="25" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E27" s="25"/>
       <c r="F27" s="25" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="G27" s="26" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="H27" s="26"/>
       <c r="I27" s="25" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="J27" s="25" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" s="28" customFormat="1" ht="45.75">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" s="28" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" s="23">
         <v>28</v>
       </c>
       <c r="B28" s="23" t="s">
+        <v>88</v>
+      </c>
+      <c r="C28" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="E28" s="24" t="s">
         <v>90</v>
       </c>
-      <c r="C28" s="23" t="s">
-        <v>18</v>
-      </c>
-      <c r="D28" s="2" t="s">
+      <c r="F28" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="G28" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="H28" s="24" t="s">
         <v>91</v>
       </c>
-      <c r="E28" s="24" t="s">
-        <v>92</v>
-      </c>
-      <c r="F28" s="23" t="s">
-        <v>20</v>
-      </c>
-      <c r="G28" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="H28" s="24" t="s">
-        <v>93</v>
-      </c>
       <c r="I28" s="23" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="J28" s="23" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" s="28" customFormat="1" ht="30.75">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" s="28" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="23">
         <v>29</v>
       </c>
       <c r="B29" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="C29" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="E29" s="24" t="s">
         <v>94</v>
       </c>
-      <c r="C29" s="23" t="s">
-        <v>18</v>
-      </c>
-      <c r="D29" s="2" t="s">
+      <c r="F29" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="G29" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="H29" s="24" t="s">
         <v>95</v>
       </c>
-      <c r="E29" s="24" t="s">
-        <v>96</v>
-      </c>
-      <c r="F29" s="23" t="s">
-        <v>20</v>
-      </c>
-      <c r="G29" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="H29" s="24" t="s">
-        <v>97</v>
-      </c>
       <c r="I29" s="23" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="J29" s="23" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" s="28" customFormat="1" ht="30.75">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" s="28" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="23">
         <v>30</v>
       </c>
       <c r="B30" s="23" t="s">
+        <v>96</v>
+      </c>
+      <c r="C30" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="E30" s="24" t="s">
         <v>98</v>
       </c>
-      <c r="C30" s="23" t="s">
-        <v>18</v>
-      </c>
-      <c r="D30" s="2" t="s">
+      <c r="F30" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="G30" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="H30" s="24" t="s">
         <v>99</v>
       </c>
-      <c r="E30" s="24" t="s">
+      <c r="I30" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="J30" s="23" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31" s="15">
+        <v>31</v>
+      </c>
+      <c r="B31" s="15" t="s">
         <v>100</v>
       </c>
-      <c r="F30" s="23" t="s">
-        <v>20</v>
-      </c>
-      <c r="G30" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="H30" s="24" t="s">
+      <c r="C31" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D31" s="2" t="s">
         <v>101</v>
-      </c>
-      <c r="I30" s="23" t="s">
-        <v>15</v>
-      </c>
-      <c r="J30" s="23" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" ht="15">
-      <c r="A31" s="15">
-        <v>31</v>
-      </c>
-      <c r="B31" s="15" t="s">
-        <v>102</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>103</v>
       </c>
       <c r="E31" s="2"/>
       <c r="F31" s="15" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="G31" s="15" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H31" s="15"/>
       <c r="I31" s="15" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J31" s="15" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" ht="15">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="15">
         <v>32</v>
       </c>
       <c r="B32" s="15" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E32" s="2"/>
       <c r="F32" s="15" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="G32" s="15" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H32" s="15"/>
       <c r="I32" s="15" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J32" s="15" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" ht="15">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="15">
         <v>33</v>
       </c>
       <c r="B33" s="15" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C33" s="15" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E33" s="2"/>
       <c r="F33" s="15" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="G33" s="15" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H33" s="15"/>
       <c r="I33" s="15" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="J33" s="15" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" ht="15">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="15">
         <v>34</v>
       </c>
       <c r="B34" s="15" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C34" s="15" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E34" s="2"/>
       <c r="F34" s="15" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="G34" s="15" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H34" s="15"/>
       <c r="I34" s="15" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J34" s="15" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" ht="15">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="15">
         <v>35</v>
       </c>
       <c r="B35" s="15" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C35" s="15" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E35" s="2"/>
       <c r="F35" s="15" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="G35" s="15" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H35" s="15"/>
       <c r="I35" s="15" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J35" s="15" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" ht="15">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="15">
         <v>36</v>
       </c>
       <c r="B36" s="15" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C36" s="15" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E36" s="2"/>
       <c r="F36" s="15" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="G36" s="15" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H36" s="15"/>
       <c r="I36" s="15" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J36" s="15" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" ht="15">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="15">
         <v>37</v>
       </c>
       <c r="B37" s="15" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C37" s="15" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E37" s="2"/>
       <c r="F37" s="15" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="G37" s="15" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H37" s="15"/>
       <c r="I37" s="15" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J37" s="15" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" ht="15">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="15">
         <v>38</v>
       </c>
       <c r="B38" t="s">
+        <v>115</v>
+      </c>
+      <c r="C38" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="E38" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="C38" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="E38" s="3" t="s">
-        <v>119</v>
-      </c>
       <c r="F38" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="H38" s="3"/>
       <c r="I38" s="15" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="J38" s="15" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" ht="15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="15">
         <v>39</v>
       </c>
       <c r="B39" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C39" s="15" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E39" s="2"/>
       <c r="F39" s="15" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="G39" s="15" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H39" s="15"/>
       <c r="I39" s="15" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J39" s="15" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" ht="15">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="15">
         <v>40</v>
       </c>
       <c r="B40" s="15" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C40" s="15" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E40" s="2"/>
       <c r="F40" s="15" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="G40" s="15" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H40" s="15"/>
       <c r="I40" s="15" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J40" s="15" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" ht="15">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>41</v>
       </c>
       <c r="B41" s="15" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C41" s="15" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E41" s="2"/>
       <c r="F41" s="15" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="G41" s="15" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H41" s="15"/>
       <c r="I41" s="15" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J41" s="15" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" ht="15">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>42</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C42" s="15" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E42" s="2"/>
       <c r="F42" s="15" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="G42" s="15" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H42" s="15"/>
       <c r="I42" s="15" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J42" s="15" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" ht="15">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>43</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C43" s="15" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="E43" s="2"/>
       <c r="F43" s="15" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="G43" s="15" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H43" s="15"/>
       <c r="I43" s="15" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J43" s="15" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" ht="15">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <v>44</v>
       </c>
       <c r="B44" t="s">
+        <v>128</v>
+      </c>
+      <c r="C44" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="E44" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="C44" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="D44" s="2" t="s">
+      <c r="F44" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G44" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H44" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="E44" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="F44" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G44" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H44" s="3" t="s">
-        <v>133</v>
-      </c>
       <c r="I44" s="15" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="J44" s="15" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" ht="15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <v>45</v>
       </c>
       <c r="B45" t="s">
+        <v>132</v>
+      </c>
+      <c r="C45" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="E45" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="C45" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="D45" s="2" t="s">
+      <c r="F45" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G45" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H45" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="E45" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="F45" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G45" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H45" s="3" t="s">
-        <v>137</v>
-      </c>
       <c r="I45" s="15" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="J45" s="15" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" ht="15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <v>46</v>
       </c>
       <c r="B46" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="C46" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="E46" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="C46" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="D46" s="2" t="s">
+      <c r="F46" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G46" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H46" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="E46" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="F46" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G46" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H46" s="3" t="s">
-        <v>141</v>
-      </c>
       <c r="I46" s="15" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="J46" s="15" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10" ht="15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
         <v>47</v>
       </c>
       <c r="B47" s="15" t="s">
+        <v>140</v>
+      </c>
+      <c r="C47" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="E47" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="C47" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="D47" s="2" t="s">
+      <c r="F47" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G47" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H47" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="E47" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="F47" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G47" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H47" s="3" t="s">
-        <v>145</v>
-      </c>
       <c r="I47" s="15" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="J47" s="15" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" s="28" customFormat="1" ht="15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="15">
         <v>48</v>
       </c>
       <c r="B48" s="23" t="s">
+        <v>144</v>
+      </c>
+      <c r="C48" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="E48" s="23" t="s">
         <v>146</v>
       </c>
-      <c r="C48" s="23" t="s">
-        <v>18</v>
-      </c>
-      <c r="D48" s="2" t="s">
+      <c r="F48" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="G48" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="H48" s="23" t="s">
         <v>147</v>
       </c>
-      <c r="E48" s="23" t="s">
-        <v>148</v>
-      </c>
-      <c r="F48" s="23" t="s">
-        <v>20</v>
-      </c>
-      <c r="G48" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="H48" s="23" t="s">
-        <v>149</v>
-      </c>
       <c r="I48" s="23" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="J48" s="23" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10" ht="15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="23">
         <v>49</v>
       </c>
       <c r="B49" s="15" t="s">
+        <v>148</v>
+      </c>
+      <c r="C49" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="F49" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G49" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H49" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="C49" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="D49" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="E49" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="F49" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G49" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H49" s="3" t="s">
-        <v>152</v>
-      </c>
       <c r="I49" s="15" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="J49" s="15" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10" s="28" customFormat="1" ht="15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="15">
         <v>50</v>
       </c>
       <c r="B50" s="23" t="s">
+        <v>151</v>
+      </c>
+      <c r="C50" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="E50" s="23" t="s">
         <v>153</v>
       </c>
-      <c r="C50" s="23" t="s">
-        <v>18</v>
-      </c>
-      <c r="D50" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="E50" s="23" t="s">
-        <v>155</v>
-      </c>
       <c r="F50" s="23" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G50" s="24" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="H50" s="24" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="I50" s="23" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="J50" s="23" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10" ht="30.75">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
         <v>51</v>
       </c>
       <c r="B51" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="F51" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G51" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H51" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="C51" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D51" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="E51" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="F51" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G51" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H51" s="3" t="s">
-        <v>158</v>
-      </c>
       <c r="I51" s="15" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="J51" s="15" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="52" spans="1:10" ht="15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
         <v>52</v>
       </c>
       <c r="B52" s="15" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E52" s="2"/>
       <c r="F52" s="15" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="G52" s="15" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H52" s="15"/>
       <c r="I52" s="15" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J52" s="15" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="53" spans="1:10" ht="15">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="15">
         <v>53</v>
       </c>
       <c r="B53" s="15" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E53" s="2"/>
       <c r="F53" s="15" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="G53" s="15" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H53" s="15"/>
       <c r="I53" s="15" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J53" s="15" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="54" spans="1:10" ht="15">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
         <v>54</v>
       </c>
       <c r="B54" s="15" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E54" s="2"/>
       <c r="F54" s="15" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="G54" s="15" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H54" s="15"/>
       <c r="I54" s="15" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J54" s="15" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="55" spans="1:10" ht="15">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
         <v>55</v>
       </c>
       <c r="B55" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E55" s="2"/>
       <c r="F55" s="15" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="G55" s="15" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H55" s="15"/>
       <c r="I55" s="15" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J55" s="15" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="56" spans="1:10" ht="15">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
         <v>56</v>
       </c>
       <c r="B56" t="s">
+        <v>165</v>
+      </c>
+      <c r="C56" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="E56" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="C56" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="D56" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="E56" s="2" t="s">
-        <v>169</v>
-      </c>
       <c r="F56" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G56" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="H56" s="2"/>
       <c r="I56" s="15" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="J56" s="15" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="57" spans="1:10" ht="15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
         <v>57</v>
       </c>
       <c r="B57" t="s">
+        <v>168</v>
+      </c>
+      <c r="C57" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="E57" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="C57" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="D57" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="E57" s="2" t="s">
-        <v>172</v>
-      </c>
       <c r="F57" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G57" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="H57" s="2"/>
       <c r="I57" s="15" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="J57" s="15" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="58" spans="1:10" ht="15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
         <v>58</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E58" s="2"/>
       <c r="F58" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G58" s="2"/>
       <c r="H58" s="2"/>
       <c r="I58" s="15" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J58" s="15" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="59" spans="1:10" ht="15">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
         <v>59</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C59" s="15" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="E59" s="2"/>
       <c r="F59" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G59" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="H59" s="2"/>
       <c r="I59" s="15" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J59" s="15" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="60" spans="1:10" ht="15">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
         <v>60</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E60" s="2"/>
       <c r="F60" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G60" s="3"/>
       <c r="H60" s="2"/>
       <c r="I60" s="15" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J60" s="15" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="61" spans="1:10" ht="15">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" s="2">
         <v>61</v>
       </c>
       <c r="B61" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="E61" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="C61" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D61" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="E61" s="2" t="s">
-        <v>181</v>
-      </c>
       <c r="F61" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G61" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="H61" s="16"/>
       <c r="I61" s="15" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="J61" s="15" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="62" spans="1:10" ht="15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" s="2">
         <v>62</v>
       </c>
       <c r="B62" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="C62" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="E62" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="C62" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="D62" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="E62" s="2" t="s">
-        <v>184</v>
-      </c>
       <c r="F62" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G62" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="H62" s="15"/>
       <c r="I62" s="15" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="J62" s="15" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="63" spans="1:10" ht="15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" s="2">
         <v>63</v>
       </c>
       <c r="B63" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="E63" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="C63" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D63" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="E63" s="2" t="s">
-        <v>187</v>
-      </c>
       <c r="F63" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G63" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="H63" s="16"/>
       <c r="I63" s="15" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="J63" s="15" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="64" spans="1:10" ht="15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" s="2">
         <v>64</v>
       </c>
       <c r="B64" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D64" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="E64" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="C64" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D64" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="E64" s="2" t="s">
-        <v>190</v>
-      </c>
       <c r="F64" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G64" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="H64" s="16"/>
       <c r="I64" s="15" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="J64" s="15" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="65" spans="1:10" ht="15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>64</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G65" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="H65" s="16"/>
       <c r="I65" s="15" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="J65" s="15" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="66" spans="1:10" ht="15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>65</v>
       </c>
       <c r="B66" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="C66" t="s">
+        <v>34</v>
+      </c>
+      <c r="D66" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="E66" s="27" t="s">
         <v>193</v>
       </c>
-      <c r="C66" t="s">
-        <v>36</v>
-      </c>
-      <c r="D66" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="E66" s="27" t="s">
-        <v>195</v>
-      </c>
       <c r="F66" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G66" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="H66" s="1"/>
       <c r="I66" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="J66" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="67" spans="1:10" ht="15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>66</v>
       </c>
       <c r="B67" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="C67" t="s">
+        <v>34</v>
+      </c>
+      <c r="D67" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="E67" s="3" t="s">
         <v>196</v>
       </c>
-      <c r="C67" t="s">
-        <v>36</v>
-      </c>
-      <c r="D67" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="E67" s="3" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="68" spans="1:10" ht="15">
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>67</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="F68" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G68" s="2"/>
       <c r="H68" s="2" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="I68" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J68" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="69" spans="1:10" ht="15">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>68</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G69" s="2"/>
       <c r="H69" s="2" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="I69" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J69" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="70" spans="1:10" ht="15">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>69</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="F70" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G70" s="2"/>
       <c r="H70" s="2"/>
       <c r="I70" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J70" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="71" spans="1:10" ht="15">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>70</v>
       </c>
       <c r="B71" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="C71" t="s">
+        <v>34</v>
+      </c>
+      <c r="D71" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="E71" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="C71" t="s">
-        <v>36</v>
-      </c>
-      <c r="D71" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="E71" s="3" t="s">
-        <v>208</v>
-      </c>
       <c r="F71" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G71" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="H71" s="1"/>
       <c r="I71" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="J71" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="72" spans="1:10" ht="15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>71</v>
       </c>
       <c r="B72" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="C72" t="s">
+        <v>34</v>
+      </c>
+      <c r="D72" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="E72" s="3" t="s">
         <v>209</v>
       </c>
-      <c r="C72" t="s">
-        <v>36</v>
-      </c>
-      <c r="D72" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="E72" s="3" t="s">
-        <v>211</v>
-      </c>
       <c r="F72" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G72" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="H72" s="1"/>
       <c r="I72" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="J72" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="73" spans="1:10" ht="15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>72</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="F73" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G73" s="2"/>
       <c r="H73" s="2"/>
       <c r="I73" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J73" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="74" spans="1:10" ht="15">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>73</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="F74" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G74" s="2"/>
       <c r="H74" s="2"/>
       <c r="I74" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J74" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="75" spans="1:10" ht="15">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>74</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F75" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G75" s="2"/>
       <c r="H75" s="2"/>
       <c r="I75" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J75" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="76" spans="1:10" ht="15">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>75</v>
       </c>
       <c r="B76" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="C76" t="s">
+        <v>34</v>
+      </c>
+      <c r="D76" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="E76" s="3" t="s">
         <v>218</v>
       </c>
-      <c r="C76" t="s">
-        <v>36</v>
-      </c>
-      <c r="D76" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="E76" s="3" t="s">
-        <v>220</v>
-      </c>
       <c r="F76" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G76" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="H76" s="1"/>
       <c r="I76" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="J76" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="77" spans="1:10" ht="15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>76</v>
       </c>
       <c r="B77" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="C77" t="s">
+        <v>34</v>
+      </c>
+      <c r="D77" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="E77" s="3" t="s">
         <v>221</v>
       </c>
-      <c r="C77" t="s">
-        <v>36</v>
-      </c>
-      <c r="D77" s="2" t="s">
-        <v>222</v>
-      </c>
-      <c r="E77" s="3" t="s">
-        <v>223</v>
-      </c>
       <c r="F77" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G77" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="H77" s="1"/>
       <c r="I77" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="J77" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="78" spans="1:10" ht="15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>77</v>
       </c>
       <c r="B78" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="C78" t="s">
+        <v>34</v>
+      </c>
+      <c r="D78" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="E78" s="3" t="s">
         <v>224</v>
       </c>
-      <c r="C78" t="s">
-        <v>36</v>
-      </c>
-      <c r="D78" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="E78" s="3" t="s">
-        <v>226</v>
-      </c>
       <c r="F78" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G78" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="H78" s="1"/>
       <c r="I78" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="J78" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="79" spans="1:10" ht="15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>78</v>
       </c>
       <c r="B79" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="C79" t="s">
+        <v>34</v>
+      </c>
+      <c r="D79" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="E79" s="3" t="s">
         <v>227</v>
       </c>
-      <c r="C79" t="s">
-        <v>36</v>
-      </c>
-      <c r="D79" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="E79" s="3" t="s">
-        <v>229</v>
-      </c>
       <c r="F79" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G79" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="H79" s="1"/>
       <c r="I79" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="J79" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="80" spans="1:10" ht="15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>79</v>
       </c>
       <c r="B80" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="C80" t="s">
+        <v>34</v>
+      </c>
+      <c r="D80" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="E80" s="3" t="s">
         <v>230</v>
       </c>
-      <c r="C80" t="s">
-        <v>36</v>
-      </c>
-      <c r="D80" s="2" t="s">
-        <v>231</v>
-      </c>
-      <c r="E80" s="3" t="s">
-        <v>232</v>
-      </c>
       <c r="F80" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G80" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="H80" s="1"/>
       <c r="I80" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="J80" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="81" spans="1:10" ht="15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>80</v>
       </c>
       <c r="B81" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="C81" t="s">
+        <v>34</v>
+      </c>
+      <c r="D81" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="E81" s="3" t="s">
         <v>233</v>
       </c>
-      <c r="C81" t="s">
-        <v>36</v>
-      </c>
-      <c r="D81" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="E81" s="3" t="s">
-        <v>235</v>
-      </c>
       <c r="F81" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G81" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="H81" s="1"/>
       <c r="I81" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="J81" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="82" spans="1:10" ht="15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>81</v>
       </c>
       <c r="B82" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="C82" t="s">
+        <v>34</v>
+      </c>
+      <c r="D82" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="E82" s="3" t="s">
         <v>236</v>
       </c>
-      <c r="C82" t="s">
-        <v>36</v>
-      </c>
-      <c r="D82" s="2" t="s">
-        <v>237</v>
-      </c>
-      <c r="E82" s="3" t="s">
-        <v>238</v>
-      </c>
       <c r="F82" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G82" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="H82" s="1"/>
       <c r="I82" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="J82" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="83" spans="1:10" ht="15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>82</v>
       </c>
       <c r="B83" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="C83" t="s">
+        <v>34</v>
+      </c>
+      <c r="D83" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="E83" s="3" t="s">
         <v>239</v>
       </c>
-      <c r="C83" t="s">
-        <v>36</v>
-      </c>
-      <c r="D83" s="2" t="s">
-        <v>240</v>
-      </c>
-      <c r="E83" s="3" t="s">
-        <v>241</v>
-      </c>
       <c r="F83" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G83" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="H83" s="1"/>
       <c r="I83" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="J83" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="84" spans="1:10" ht="15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>83</v>
       </c>
       <c r="B84" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="C84" t="s">
+        <v>34</v>
+      </c>
+      <c r="D84" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="E84" s="3" t="s">
         <v>242</v>
       </c>
-      <c r="C84" t="s">
-        <v>36</v>
-      </c>
-      <c r="D84" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="E84" s="3" t="s">
-        <v>244</v>
-      </c>
       <c r="F84" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G84" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="H84" s="1"/>
       <c r="I84" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="J84" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="85" spans="1:10" ht="15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>84</v>
       </c>
       <c r="B85" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="C85" t="s">
+        <v>34</v>
+      </c>
+      <c r="D85" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="E85" s="3" t="s">
         <v>245</v>
       </c>
-      <c r="C85" t="s">
-        <v>36</v>
-      </c>
-      <c r="D85" s="2" t="s">
-        <v>246</v>
-      </c>
-      <c r="E85" s="3" t="s">
-        <v>247</v>
-      </c>
       <c r="F85" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G85" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="H85" s="1"/>
       <c r="I85" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="J85" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="86" spans="1:10" ht="15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>85</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="F86" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G86" s="2"/>
       <c r="H86" s="2"/>
       <c r="I86" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J86" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="87" spans="1:10" ht="15">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>86</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="F87" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G87" s="2"/>
       <c r="H87" s="2"/>
       <c r="I87" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J87" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="88" spans="1:10" ht="15">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>87</v>
       </c>
       <c r="B88" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="C88" t="s">
+        <v>34</v>
+      </c>
+      <c r="D88" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="E88" s="4" t="s">
         <v>252</v>
       </c>
-      <c r="C88" t="s">
-        <v>36</v>
-      </c>
-      <c r="D88" s="2" t="s">
-        <v>253</v>
-      </c>
-      <c r="E88" s="4" t="s">
-        <v>254</v>
-      </c>
       <c r="F88" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G88" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="H88" s="1"/>
       <c r="I88" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="J88" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="89" spans="1:10" ht="15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>88</v>
       </c>
       <c r="B89" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="C89" t="s">
+        <v>34</v>
+      </c>
+      <c r="D89" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="E89" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="C89" t="s">
-        <v>36</v>
-      </c>
-      <c r="D89" s="2" t="s">
-        <v>256</v>
-      </c>
-      <c r="E89" s="2" t="s">
-        <v>257</v>
-      </c>
       <c r="F89" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G89" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="H89" s="1"/>
       <c r="I89" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="J89" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="90" spans="1:10" ht="15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>89</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="E90" s="2"/>
       <c r="F90" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G90" s="2"/>
       <c r="H90" s="2"/>
       <c r="I90" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J90" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="91" spans="1:10" ht="15">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>90</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="E91" s="2"/>
       <c r="F91" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G91" s="2"/>
       <c r="H91" s="2"/>
       <c r="I91" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J91" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="92" spans="1:10" ht="15">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>91</v>
       </c>
       <c r="B92" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="C92" t="s">
+        <v>34</v>
+      </c>
+      <c r="D92" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="E92" s="2" t="s">
         <v>262</v>
       </c>
-      <c r="C92" t="s">
-        <v>36</v>
-      </c>
-      <c r="D92" s="2" t="s">
-        <v>263</v>
-      </c>
-      <c r="E92" s="2" t="s">
-        <v>264</v>
-      </c>
       <c r="F92" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G92" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="H92" s="1"/>
       <c r="I92" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="J92" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="93" spans="1:10" ht="15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>92</v>
       </c>
       <c r="B93" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="C93" t="s">
+        <v>34</v>
+      </c>
+      <c r="D93" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="E93" s="2" t="s">
         <v>265</v>
       </c>
-      <c r="C93" t="s">
-        <v>36</v>
-      </c>
-      <c r="D93" s="2" t="s">
+      <c r="F93" s="1" t="s">
         <v>266</v>
       </c>
-      <c r="E93" s="2" t="s">
+      <c r="G93" s="1" t="s">
         <v>267</v>
-      </c>
-      <c r="F93" s="1" t="s">
-        <v>268</v>
-      </c>
-      <c r="G93" s="1" t="s">
-        <v>269</v>
       </c>
       <c r="H93" s="1"/>
       <c r="I93" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="J93" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="94" spans="1:10" ht="121.5">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>93</v>
       </c>
       <c r="B94" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="C94" t="s">
+        <v>34</v>
+      </c>
+      <c r="D94" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="E94" s="13" t="s">
         <v>270</v>
       </c>
-      <c r="C94" t="s">
-        <v>36</v>
-      </c>
-      <c r="D94" s="2" t="s">
+      <c r="F94" s="6" t="s">
         <v>271</v>
       </c>
-      <c r="E94" s="13" t="s">
+      <c r="G94" s="7" t="s">
         <v>272</v>
-      </c>
-      <c r="F94" s="6" t="s">
-        <v>273</v>
-      </c>
-      <c r="G94" s="7" t="s">
-        <v>274</v>
       </c>
       <c r="H94" s="12"/>
       <c r="I94" s="6" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="J94" s="6" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="95" spans="1:10" ht="45.75">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>94</v>
       </c>
       <c r="B95" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="C95" t="s">
+        <v>34</v>
+      </c>
+      <c r="D95" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="E95" s="10" t="s">
         <v>277</v>
       </c>
-      <c r="C95" t="s">
-        <v>36</v>
-      </c>
-      <c r="D95" s="2" t="s">
+      <c r="F95" s="10" t="s">
+        <v>271</v>
+      </c>
+      <c r="G95" s="5" t="s">
         <v>278</v>
       </c>
-      <c r="E95" s="10" t="s">
-        <v>279</v>
-      </c>
-      <c r="F95" s="10" t="s">
+      <c r="I95" s="10" t="s">
         <v>273</v>
       </c>
-      <c r="G95" s="5" t="s">
-        <v>280</v>
-      </c>
-      <c r="I95" s="10" t="s">
-        <v>275</v>
-      </c>
       <c r="J95" s="10" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="96" spans="1:10" ht="15">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>95</v>
       </c>
       <c r="B96" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="C96" t="s">
+        <v>34</v>
+      </c>
+      <c r="D96" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="E96" s="14" t="s">
         <v>281</v>
       </c>
-      <c r="C96" t="s">
-        <v>36</v>
-      </c>
-      <c r="D96" s="2" t="s">
+      <c r="F96" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="G96" s="14" t="s">
         <v>282</v>
       </c>
-      <c r="E96" s="14" t="s">
-        <v>283</v>
-      </c>
-      <c r="F96" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="G96" s="14" t="s">
-        <v>284</v>
-      </c>
       <c r="I96" s="10" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="J96" s="10" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="97" spans="1:10" ht="45.75">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>96</v>
       </c>
       <c r="B97" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="C97" t="s">
+        <v>34</v>
+      </c>
+      <c r="D97" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="E97" t="s">
         <v>285</v>
       </c>
-      <c r="C97" t="s">
-        <v>36</v>
-      </c>
-      <c r="D97" s="2" t="s">
+      <c r="F97" s="10" t="s">
+        <v>271</v>
+      </c>
+      <c r="G97" s="5" t="s">
         <v>286</v>
       </c>
-      <c r="E97" t="s">
-        <v>287</v>
-      </c>
-      <c r="F97" s="10" t="s">
+      <c r="I97" s="10" t="s">
         <v>273</v>
       </c>
-      <c r="G97" s="5" t="s">
-        <v>288</v>
-      </c>
-      <c r="I97" s="10" t="s">
-        <v>275</v>
-      </c>
       <c r="J97" s="10" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="98" spans="1:10" ht="15">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>97</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="C98" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D98" s="2" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="F98" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="I98" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J98" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="99" spans="1:10" ht="259.5">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" ht="255" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>98</v>
       </c>
       <c r="B99" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="C99" t="s">
+        <v>34</v>
+      </c>
+      <c r="D99" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="E99" s="5" t="s">
         <v>291</v>
       </c>
-      <c r="C99" t="s">
-        <v>36</v>
-      </c>
-      <c r="D99" s="2" t="s">
+      <c r="F99" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="G99" s="7" t="s">
         <v>292</v>
       </c>
-      <c r="E99" s="5" t="s">
-        <v>293</v>
-      </c>
-      <c r="F99" s="6" t="s">
+      <c r="I99" s="6" t="s">
         <v>273</v>
       </c>
-      <c r="G99" s="7" t="s">
-        <v>294</v>
-      </c>
-      <c r="I99" s="6" t="s">
-        <v>275</v>
-      </c>
       <c r="J99" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="100" spans="1:10" ht="15">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>99</v>
       </c>
       <c r="B100" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="C100" t="s">
+        <v>34</v>
+      </c>
+      <c r="D100" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="E100" s="8" t="s">
         <v>295</v>
       </c>
-      <c r="C100" t="s">
-        <v>36</v>
-      </c>
-      <c r="D100" s="2" t="s">
+      <c r="F100" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G100" s="9" t="s">
         <v>296</v>
       </c>
-      <c r="E100" s="8" t="s">
-        <v>297</v>
-      </c>
-      <c r="F100" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="G100" s="9" t="s">
-        <v>298</v>
-      </c>
       <c r="I100" s="6" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="J100" s="6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="101" spans="1:10" ht="396.75">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" ht="390" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>100</v>
       </c>
       <c r="B101" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="C101" t="s">
+        <v>34</v>
+      </c>
+      <c r="D101" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="E101" s="29" t="s">
         <v>299</v>
       </c>
-      <c r="C101" t="s">
-        <v>36</v>
-      </c>
-      <c r="D101" s="2" t="s">
+      <c r="F101" s="10" t="s">
+        <v>271</v>
+      </c>
+      <c r="G101" s="5" t="s">
         <v>300</v>
       </c>
-      <c r="E101" s="33" t="s">
-        <v>301</v>
-      </c>
-      <c r="F101" s="10" t="s">
+      <c r="I101" s="10" t="s">
         <v>273</v>
       </c>
-      <c r="G101" s="5" t="s">
-        <v>302</v>
-      </c>
-      <c r="I101" s="10" t="s">
-        <v>275</v>
-      </c>
       <c r="J101" s="10" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="102" spans="1:10" ht="106.5">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" ht="105" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>101</v>
       </c>
       <c r="B102" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="C102" t="s">
+        <v>34</v>
+      </c>
+      <c r="D102" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="E102" s="11" t="s">
         <v>303</v>
       </c>
-      <c r="C102" t="s">
-        <v>36</v>
-      </c>
-      <c r="D102" s="2" t="s">
+      <c r="F102" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="G102" s="12" t="s">
         <v>304</v>
       </c>
-      <c r="E102" s="11" t="s">
-        <v>305</v>
-      </c>
-      <c r="F102" s="6" t="s">
+      <c r="I102" s="6" t="s">
         <v>273</v>
       </c>
-      <c r="G102" s="12" t="s">
-        <v>306</v>
-      </c>
-      <c r="I102" s="6" t="s">
-        <v>275</v>
-      </c>
       <c r="J102" s="6" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="103" spans="1:10" ht="106.5">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" ht="105" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>102</v>
       </c>
       <c r="B103" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="C103" t="s">
+        <v>34</v>
+      </c>
+      <c r="D103" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="E103" s="5" t="s">
         <v>307</v>
       </c>
-      <c r="C103" t="s">
-        <v>36</v>
-      </c>
-      <c r="D103" s="2" t="s">
+      <c r="F103" s="10" t="s">
+        <v>271</v>
+      </c>
+      <c r="G103" s="5" t="s">
         <v>308</v>
       </c>
-      <c r="E103" s="5" t="s">
-        <v>309</v>
-      </c>
-      <c r="F103" s="10" t="s">
+      <c r="I103" s="6" t="s">
         <v>273</v>
       </c>
-      <c r="G103" s="5" t="s">
-        <v>310</v>
-      </c>
-      <c r="I103" s="6" t="s">
-        <v>275</v>
-      </c>
       <c r="J103" s="10" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="104" spans="1:10" ht="30.75">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>103</v>
       </c>
       <c r="B104" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="C104" t="s">
+        <v>34</v>
+      </c>
+      <c r="D104" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="E104" t="s">
         <v>311</v>
       </c>
-      <c r="C104" t="s">
-        <v>36</v>
-      </c>
-      <c r="D104" s="2" t="s">
+      <c r="F104" s="10" t="s">
+        <v>271</v>
+      </c>
+      <c r="G104" s="12" t="s">
         <v>312</v>
       </c>
-      <c r="E104" t="s">
-        <v>313</v>
-      </c>
-      <c r="F104" s="10" t="s">
+      <c r="I104" s="10" t="s">
         <v>273</v>
       </c>
-      <c r="G104" s="12" t="s">
-        <v>314</v>
-      </c>
-      <c r="I104" s="10" t="s">
-        <v>275</v>
-      </c>
       <c r="J104" s="10" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="105" spans="1:10" ht="15">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>104</v>
       </c>
       <c r="B105" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="C105" t="s">
+        <v>34</v>
+      </c>
+      <c r="D105" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="E105" s="14" t="s">
         <v>315</v>
       </c>
-      <c r="C105" t="s">
-        <v>36</v>
-      </c>
-      <c r="D105" s="2" t="s">
+      <c r="F105" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="G105" s="14" t="s">
         <v>316</v>
       </c>
-      <c r="E105" s="14" t="s">
-        <v>317</v>
-      </c>
-      <c r="F105" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="G105" s="14" t="s">
-        <v>318</v>
-      </c>
       <c r="I105" s="10" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="J105" s="10" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -4590,6 +4565,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100B1DC67C611DD5E4D81775F9F3E26A7B2" ma:contentTypeVersion="16" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="7f379a5812b480a74f9d031be5f88a83">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xmlns:ns3="12535b08-222e-45d2-b6db-15019f1afee6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="dbce1e37d7de67e1c835013ca0ee7a7c" ns2:_="" ns3:_="">
     <xsd:import namespace="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
@@ -4830,15 +4814,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -4852,13 +4827,39 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{94761517-FE09-4464-B96F-D998528E68DF}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{362E0444-0B0C-4DF9-8194-BB08BDB29ECB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{362E0444-0B0C-4DF9-8194-BB08BDB29ECB}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{94761517-FE09-4464-B96F-D998528E68DF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
+    <ds:schemaRef ds:uri="12535b08-222e-45d2-b6db-15019f1afee6"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DFED9ACA-827C-4B16-98B6-54E8085DB47D}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DFED9ACA-827C-4B16-98B6-54E8085DB47D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
+    <ds:schemaRef ds:uri="12535b08-222e-45d2-b6db-15019f1afee6"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
correct the total sugar variable
</commit_message>
<xml_diff>
--- a/rmonize/data_proc_elem/DPE_KORA_S3_P2.xlsx
+++ b/rmonize/data_proc_elem/DPE_KORA_S3_P2.xlsx
@@ -1119,13 +1119,13 @@
     <t>Total fruit intake [g/d]</t>
   </si>
   <si>
-    <t>dkmosa + dkdisa</t>
-  </si>
-  <si>
-    <t>dkmosa (monosaccharides) + dkdisa (disaccharides)</t>
-  </si>
-  <si>
-    <t>dkmosa; dkdisa</t>
+    <t>dmosa (monosaccharides) + ddisa (disaccharides)</t>
+  </si>
+  <si>
+    <t>dmosa + ddisa</t>
+  </si>
+  <si>
+    <t>dmosa; ddisa</t>
   </si>
 </sst>
 </file>
@@ -1691,7 +1691,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A70" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F88" sqref="F88"/>
+      <selection pane="bottomLeft" activeCell="F84" sqref="F84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -4655,10 +4655,10 @@
         <v>270</v>
       </c>
       <c r="H88" s="24" t="s">
+        <v>349</v>
+      </c>
+      <c r="I88" s="24" t="s">
         <v>348</v>
-      </c>
-      <c r="I88" s="24" t="s">
-        <v>349</v>
       </c>
       <c r="J88" s="17" t="s">
         <v>277</v>
@@ -5379,6 +5379,27 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Zeit xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="12535b08-222e-45d2-b6db-15019f1afee6" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100B1DC67C611DD5E4D81775F9F3E26A7B2" ma:contentTypeVersion="16" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="7f379a5812b480a74f9d031be5f88a83">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xmlns:ns3="12535b08-222e-45d2-b6db-15019f1afee6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="dbce1e37d7de67e1c835013ca0ee7a7c" ns2:_="" ns3:_="">
     <xsd:import namespace="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
@@ -5619,28 +5640,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DFED9ACA-827C-4B16-98B6-54E8085DB47D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
+    <ds:schemaRef ds:uri="12535b08-222e-45d2-b6db-15019f1afee6"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Zeit xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="12535b08-222e-45d2-b6db-15019f1afee6" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{362E0444-0B0C-4DF9-8194-BB08BDB29ECB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{05EDAC75-43D1-4B55-97A0-34C880419949}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5657,29 +5682,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{362E0444-0B0C-4DF9-8194-BB08BDB29ECB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DFED9ACA-827C-4B16-98B6-54E8085DB47D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
-    <ds:schemaRef ds:uri="12535b08-222e-45d2-b6db-15019f1afee6"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
correction of the Mlst_harmo::algorithm for the sugar variables
</commit_message>
<xml_diff>
--- a/rmonize/data_proc_elem/DPE_KORA_S3_P2.xlsx
+++ b/rmonize/data_proc_elem/DPE_KORA_S3_P2.xlsx
@@ -1119,13 +1119,13 @@
     <t>Total fruit intake [g/d]</t>
   </si>
   <si>
-    <t>dmosa + ddisa</t>
-  </si>
-  <si>
     <t>dkmosa; dkdisa</t>
   </si>
   <si>
     <t>dkmosa (monosaccharides) + dkdisa (disaccharides)</t>
+  </si>
+  <si>
+    <t>dkmosa + dkdisa</t>
   </si>
 </sst>
 </file>
@@ -1691,7 +1691,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A70" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I87" sqref="I87"/>
+      <selection pane="bottomLeft" activeCell="H88" sqref="H88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -4649,16 +4649,16 @@
         <v>14</v>
       </c>
       <c r="F88" s="24" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="G88" s="24" t="s">
         <v>270</v>
       </c>
       <c r="H88" s="24" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="I88" s="24" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="J88" s="17" t="s">
         <v>277</v>
@@ -5379,6 +5379,27 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Zeit xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="12535b08-222e-45d2-b6db-15019f1afee6" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100B1DC67C611DD5E4D81775F9F3E26A7B2" ma:contentTypeVersion="16" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="7f379a5812b480a74f9d031be5f88a83">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xmlns:ns3="12535b08-222e-45d2-b6db-15019f1afee6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="dbce1e37d7de67e1c835013ca0ee7a7c" ns2:_="" ns3:_="">
     <xsd:import namespace="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
@@ -5619,28 +5640,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DFED9ACA-827C-4B16-98B6-54E8085DB47D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
+    <ds:schemaRef ds:uri="12535b08-222e-45d2-b6db-15019f1afee6"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Zeit xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="12535b08-222e-45d2-b6db-15019f1afee6" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{362E0444-0B0C-4DF9-8194-BB08BDB29ECB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{05EDAC75-43D1-4B55-97A0-34C880419949}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5657,29 +5682,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{362E0444-0B0C-4DF9-8194-BB08BDB29ECB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DFED9ACA-827C-4B16-98B6-54E8085DB47D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
-    <ds:schemaRef ds:uri="12535b08-222e-45d2-b6db-15019f1afee6"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>